<commit_message>
coisinha amais em excel
</commit_message>
<xml_diff>
--- a/BaseLimpo/2019_coleta_tipos_residuos.xlsx
+++ b/BaseLimpo/2019_coleta_tipos_residuos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1796,92 +1796,46 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Total Geral</t>
+          <t>Desconsiderando Escoria, Chorume, Cancelamentos E Saï¿½Das De Resï¿½Duos</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>466.713</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>438.849</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>474.52</v>
+        <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>480.571</v>
+        <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>479.302</v>
+        <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>433.342</v>
+        <v>0</v>
       </c>
       <c r="H30" t="n">
-        <v>469.116</v>
+        <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>468.325</v>
+        <v>0</v>
       </c>
       <c r="J30" t="n">
-        <v>459.441</v>
+        <v>0</v>
       </c>
       <c r="K30" t="n">
-        <v>484.437</v>
+        <v>0</v>
       </c>
       <c r="L30" t="n">
-        <v>467.288</v>
+        <v>0</v>
       </c>
       <c r="M30" t="n">
-        <v>507.177</v>
+        <v>0</v>
       </c>
       <c r="N30" t="n">
-        <v>5629.081</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Desconsiderando Escoria, Chorume, Cancelamentos E Saï¿½Das De Resï¿½Duos</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>0</v>
-      </c>
-      <c r="C31" t="n">
-        <v>0</v>
-      </c>
-      <c r="D31" t="n">
-        <v>0</v>
-      </c>
-      <c r="E31" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" t="n">
-        <v>0</v>
-      </c>
-      <c r="G31" t="n">
-        <v>0</v>
-      </c>
-      <c r="H31" t="n">
-        <v>0</v>
-      </c>
-      <c r="I31" t="n">
-        <v>0</v>
-      </c>
-      <c r="J31" t="n">
-        <v>0</v>
-      </c>
-      <c r="K31" t="n">
-        <v>0</v>
-      </c>
-      <c r="L31" t="n">
-        <v>0</v>
-      </c>
-      <c r="M31" t="n">
-        <v>0</v>
-      </c>
-      <c r="N31" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
solução para 2019 e 2020
</commit_message>
<xml_diff>
--- a/BaseLimpo/2019_coleta_tipos_residuos.xlsx
+++ b/BaseLimpo/2019_coleta_tipos_residuos.xlsx
@@ -512,43 +512,43 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>326.387</v>
+        <v>326387</v>
       </c>
       <c r="C2" t="n">
-        <v>292.481</v>
+        <v>292481</v>
       </c>
       <c r="D2" t="n">
-        <v>314.108</v>
+        <v>314108</v>
       </c>
       <c r="E2" t="n">
-        <v>313.198</v>
+        <v>313198</v>
       </c>
       <c r="F2" t="n">
-        <v>307.805</v>
+        <v>307805</v>
       </c>
       <c r="G2" t="n">
-        <v>284.772</v>
+        <v>284772</v>
       </c>
       <c r="H2" t="n">
-        <v>302.068</v>
+        <v>302068</v>
       </c>
       <c r="I2" t="n">
-        <v>295.446</v>
+        <v>295446</v>
       </c>
       <c r="J2" t="n">
-        <v>292.653</v>
+        <v>292653</v>
       </c>
       <c r="K2" t="n">
-        <v>316.233</v>
+        <v>316233</v>
       </c>
       <c r="L2" t="n">
-        <v>302.574</v>
+        <v>302574</v>
       </c>
       <c r="M2" t="n">
-        <v>332.356</v>
+        <v>332356</v>
       </c>
       <c r="N2" t="n">
-        <v>3680.081</v>
+        <v>3680081</v>
       </c>
     </row>
     <row r="3">
@@ -558,43 +558,43 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>24.343</v>
+        <v>24343</v>
       </c>
       <c r="C3" t="n">
-        <v>21.038</v>
+        <v>21038</v>
       </c>
       <c r="D3" t="n">
-        <v>24.972</v>
+        <v>24972</v>
       </c>
       <c r="E3" t="n">
-        <v>27.29</v>
+        <v>27290</v>
       </c>
       <c r="F3" t="n">
-        <v>26.278</v>
+        <v>26278</v>
       </c>
       <c r="G3" t="n">
-        <v>14.652</v>
+        <v>14652</v>
       </c>
       <c r="H3" t="n">
-        <v>19.44</v>
+        <v>19440</v>
       </c>
       <c r="I3" t="n">
-        <v>20.496</v>
+        <v>20496</v>
       </c>
       <c r="J3" t="n">
-        <v>16.979</v>
+        <v>16979</v>
       </c>
       <c r="K3" t="n">
-        <v>15.918</v>
+        <v>15918</v>
       </c>
       <c r="L3" t="n">
-        <v>11.188</v>
+        <v>11188</v>
       </c>
       <c r="M3" t="n">
-        <v>11.945</v>
+        <v>11945</v>
       </c>
       <c r="N3" t="n">
-        <v>234.539</v>
+        <v>234539</v>
       </c>
     </row>
     <row r="4">
@@ -604,43 +604,43 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>36.532</v>
+        <v>36532</v>
       </c>
       <c r="C4" t="n">
-        <v>36.992</v>
+        <v>36992</v>
       </c>
       <c r="D4" t="n">
-        <v>38.227</v>
+        <v>38227</v>
       </c>
       <c r="E4" t="n">
-        <v>40.459</v>
+        <v>40459</v>
       </c>
       <c r="F4" t="n">
-        <v>40.148</v>
+        <v>40148</v>
       </c>
       <c r="G4" t="n">
-        <v>28.873</v>
+        <v>28873</v>
       </c>
       <c r="H4" t="n">
-        <v>36.623</v>
+        <v>36623</v>
       </c>
       <c r="I4" t="n">
-        <v>38.352</v>
+        <v>38352</v>
       </c>
       <c r="J4" t="n">
-        <v>36.974</v>
+        <v>36974</v>
       </c>
       <c r="K4" t="n">
-        <v>42.03</v>
+        <v>42030</v>
       </c>
       <c r="L4" t="n">
-        <v>38.401</v>
+        <v>38401</v>
       </c>
       <c r="M4" t="n">
-        <v>34.125</v>
+        <v>34125</v>
       </c>
       <c r="N4" t="n">
-        <v>447.7359999999999</v>
+        <v>447736</v>
       </c>
     </row>
     <row r="5">
@@ -650,43 +650,43 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>17.128</v>
+        <v>17128</v>
       </c>
       <c r="C5" t="n">
-        <v>17.363</v>
+        <v>17363</v>
       </c>
       <c r="D5" t="n">
-        <v>19.584</v>
+        <v>19584</v>
       </c>
       <c r="E5" t="n">
-        <v>18.609</v>
+        <v>18609</v>
       </c>
       <c r="F5" t="n">
-        <v>18.258</v>
+        <v>18258</v>
       </c>
       <c r="G5" t="n">
-        <v>22.252</v>
+        <v>22252</v>
       </c>
       <c r="H5" t="n">
-        <v>19.119</v>
+        <v>19119</v>
       </c>
       <c r="I5" t="n">
-        <v>19.711</v>
+        <v>19711</v>
       </c>
       <c r="J5" t="n">
-        <v>26.336</v>
+        <v>26336</v>
       </c>
       <c r="K5" t="n">
-        <v>23.936</v>
+        <v>23936</v>
       </c>
       <c r="L5" t="n">
-        <v>24.282</v>
+        <v>24282</v>
       </c>
       <c r="M5" t="n">
-        <v>28.839</v>
+        <v>28839</v>
       </c>
       <c r="N5" t="n">
-        <v>255.417</v>
+        <v>255417</v>
       </c>
     </row>
     <row r="6">
@@ -696,43 +696,43 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7.217</v>
+        <v>7217</v>
       </c>
       <c r="C6" t="n">
-        <v>19.335</v>
+        <v>19335</v>
       </c>
       <c r="D6" t="n">
-        <v>17.412</v>
+        <v>17412</v>
       </c>
       <c r="E6" t="n">
-        <v>13.491</v>
+        <v>13491</v>
       </c>
       <c r="F6" t="n">
-        <v>19.251</v>
+        <v>19251</v>
       </c>
       <c r="G6" t="n">
-        <v>16.131</v>
+        <v>16131</v>
       </c>
       <c r="H6" t="n">
-        <v>20.046</v>
+        <v>20046</v>
       </c>
       <c r="I6" t="n">
-        <v>17.582</v>
+        <v>17582</v>
       </c>
       <c r="J6" t="n">
-        <v>17.344</v>
+        <v>17344</v>
       </c>
       <c r="K6" t="n">
-        <v>20.299</v>
+        <v>20299</v>
       </c>
       <c r="L6" t="n">
-        <v>16.931</v>
+        <v>16931</v>
       </c>
       <c r="M6" t="n">
-        <v>15.946</v>
+        <v>15946</v>
       </c>
       <c r="N6" t="n">
-        <v>200.985</v>
+        <v>200985</v>
       </c>
     </row>
     <row r="7">
@@ -742,43 +742,43 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>15.317</v>
+        <v>15317</v>
       </c>
       <c r="C7" t="n">
-        <v>14.421</v>
+        <v>14421</v>
       </c>
       <c r="D7" t="n">
-        <v>14.85</v>
+        <v>14850</v>
       </c>
       <c r="E7" t="n">
-        <v>18.373</v>
+        <v>18373</v>
       </c>
       <c r="F7" t="n">
-        <v>16.362</v>
+        <v>16362</v>
       </c>
       <c r="G7" t="n">
-        <v>16.696</v>
+        <v>16696</v>
       </c>
       <c r="H7" t="n">
-        <v>15.999</v>
+        <v>15999</v>
       </c>
       <c r="I7" t="n">
-        <v>16.723</v>
+        <v>16723</v>
       </c>
       <c r="J7" t="n">
-        <v>14.182</v>
+        <v>14182</v>
       </c>
       <c r="K7" t="n">
-        <v>16.41</v>
+        <v>16410</v>
       </c>
       <c r="L7" t="n">
-        <v>16.483</v>
+        <v>16483</v>
       </c>
       <c r="M7" t="n">
-        <v>13.552</v>
+        <v>13552</v>
       </c>
       <c r="N7" t="n">
-        <v>189.368</v>
+        <v>189368</v>
       </c>
     </row>
     <row r="8">
@@ -788,43 +788,43 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>6.97</v>
+        <v>6970</v>
       </c>
       <c r="C8" t="n">
-        <v>7.003</v>
+        <v>7003</v>
       </c>
       <c r="D8" t="n">
-        <v>11.414</v>
+        <v>11414</v>
       </c>
       <c r="E8" t="n">
-        <v>16.388</v>
+        <v>16388</v>
       </c>
       <c r="F8" t="n">
-        <v>18.673</v>
+        <v>18673</v>
       </c>
       <c r="G8" t="n">
-        <v>20.9</v>
+        <v>20900</v>
       </c>
       <c r="H8" t="n">
-        <v>21.377</v>
+        <v>21377</v>
       </c>
       <c r="I8" t="n">
-        <v>21.668</v>
+        <v>21668</v>
       </c>
       <c r="J8" t="n">
-        <v>19.402</v>
+        <v>19402</v>
       </c>
       <c r="K8" t="n">
-        <v>14.215</v>
+        <v>14215</v>
       </c>
       <c r="L8" t="n">
-        <v>24.054</v>
+        <v>24054</v>
       </c>
       <c r="M8" t="n">
-        <v>36.291</v>
+        <v>36291</v>
       </c>
       <c r="N8" t="n">
-        <v>218.355</v>
+        <v>218355</v>
       </c>
     </row>
     <row r="9">
@@ -834,43 +834,43 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>6.699</v>
+        <v>6699</v>
       </c>
       <c r="C9" t="n">
-        <v>6.26</v>
+        <v>6260</v>
       </c>
       <c r="D9" t="n">
-        <v>7.951</v>
+        <v>7951</v>
       </c>
       <c r="E9" t="n">
-        <v>7.762</v>
+        <v>7762</v>
       </c>
       <c r="F9" t="n">
-        <v>6.688</v>
+        <v>6688</v>
       </c>
       <c r="G9" t="n">
-        <v>6.517</v>
+        <v>6517</v>
       </c>
       <c r="H9" t="n">
-        <v>7.616</v>
+        <v>7616</v>
       </c>
       <c r="I9" t="n">
-        <v>8.714</v>
+        <v>8714</v>
       </c>
       <c r="J9" t="n">
-        <v>7.783</v>
+        <v>7783</v>
       </c>
       <c r="K9" t="n">
-        <v>5.716</v>
+        <v>5716</v>
       </c>
       <c r="L9" t="n">
-        <v>5.096</v>
+        <v>5096</v>
       </c>
       <c r="M9" t="n">
-        <v>5.061</v>
+        <v>5061</v>
       </c>
       <c r="N9" t="n">
-        <v>81.863</v>
+        <v>81863</v>
       </c>
     </row>
     <row r="10">
@@ -880,43 +880,43 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>7.441</v>
+        <v>7441</v>
       </c>
       <c r="C10" t="n">
-        <v>6.524</v>
+        <v>6524</v>
       </c>
       <c r="D10" t="n">
-        <v>6.724</v>
+        <v>6724</v>
       </c>
       <c r="E10" t="n">
-        <v>6.483</v>
+        <v>6483</v>
       </c>
       <c r="F10" t="n">
-        <v>6.391</v>
+        <v>6391</v>
       </c>
       <c r="G10" t="n">
-        <v>5.799</v>
+        <v>5799</v>
       </c>
       <c r="H10" t="n">
-        <v>6.511</v>
+        <v>6511</v>
       </c>
       <c r="I10" t="n">
-        <v>6.415</v>
+        <v>6415</v>
       </c>
       <c r="J10" t="n">
-        <v>6.436</v>
+        <v>6436</v>
       </c>
       <c r="K10" t="n">
-        <v>6.877</v>
+        <v>6877</v>
       </c>
       <c r="L10" t="n">
-        <v>6.791</v>
+        <v>6791</v>
       </c>
       <c r="M10" t="n">
-        <v>8.061999999999999</v>
+        <v>8062</v>
       </c>
       <c r="N10" t="n">
-        <v>80.45399999999999</v>
+        <v>80454</v>
       </c>
     </row>
     <row r="11">
@@ -926,43 +926,43 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>5.404</v>
+        <v>5404</v>
       </c>
       <c r="C11" t="n">
-        <v>5.01</v>
+        <v>5010</v>
       </c>
       <c r="D11" t="n">
-        <v>5.548</v>
+        <v>5548</v>
       </c>
       <c r="E11" t="n">
-        <v>4.693</v>
+        <v>4693</v>
       </c>
       <c r="F11" t="n">
-        <v>5.348</v>
+        <v>5348</v>
       </c>
       <c r="G11" t="n">
-        <v>4.415</v>
+        <v>4415</v>
       </c>
       <c r="H11" t="n">
-        <v>6.01</v>
+        <v>6010</v>
       </c>
       <c r="I11" t="n">
-        <v>5.281</v>
+        <v>5281</v>
       </c>
       <c r="J11" t="n">
-        <v>5.897</v>
+        <v>5897</v>
       </c>
       <c r="K11" t="n">
-        <v>5.85</v>
+        <v>5850</v>
       </c>
       <c r="L11" t="n">
-        <v>5.963</v>
+        <v>5963</v>
       </c>
       <c r="M11" t="n">
-        <v>5.906</v>
+        <v>5906</v>
       </c>
       <c r="N11" t="n">
-        <v>65.325</v>
+        <v>65325</v>
       </c>
     </row>
     <row r="12">
@@ -972,43 +972,43 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>3.634</v>
+        <v>3634</v>
       </c>
       <c r="C12" t="n">
-        <v>3.358</v>
+        <v>3358</v>
       </c>
       <c r="D12" t="n">
-        <v>3.782</v>
+        <v>3782</v>
       </c>
       <c r="E12" t="n">
-        <v>3.943</v>
+        <v>3943</v>
       </c>
       <c r="F12" t="n">
-        <v>3.787</v>
+        <v>3787</v>
       </c>
       <c r="G12" t="n">
-        <v>2.831</v>
+        <v>2831</v>
       </c>
       <c r="H12" t="n">
-        <v>3.261</v>
+        <v>3261</v>
       </c>
       <c r="I12" t="n">
-        <v>3.546</v>
+        <v>3546</v>
       </c>
       <c r="J12" t="n">
-        <v>2.886</v>
+        <v>2886</v>
       </c>
       <c r="K12" t="n">
-        <v>2.656</v>
+        <v>2656</v>
       </c>
       <c r="L12" t="n">
-        <v>2.253</v>
+        <v>2253</v>
       </c>
       <c r="M12" t="n">
-        <v>2.027</v>
+        <v>2027</v>
       </c>
       <c r="N12" t="n">
-        <v>37.964</v>
+        <v>37964</v>
       </c>
     </row>
     <row r="13">
@@ -1018,43 +1018,43 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>3.979</v>
+        <v>3979</v>
       </c>
       <c r="C13" t="n">
-        <v>4.103</v>
+        <v>4103</v>
       </c>
       <c r="D13" t="n">
-        <v>4.3</v>
+        <v>4300</v>
       </c>
       <c r="E13" t="n">
-        <v>3.973</v>
+        <v>3973</v>
       </c>
       <c r="F13" t="n">
-        <v>4.391</v>
+        <v>4391</v>
       </c>
       <c r="G13" t="n">
-        <v>3.812</v>
+        <v>3812</v>
       </c>
       <c r="H13" t="n">
-        <v>3.749</v>
+        <v>3749</v>
       </c>
       <c r="I13" t="n">
-        <v>3.872</v>
+        <v>3872</v>
       </c>
       <c r="J13" t="n">
-        <v>3.924</v>
+        <v>3924</v>
       </c>
       <c r="K13" t="n">
-        <v>5.108</v>
+        <v>5108</v>
       </c>
       <c r="L13" t="n">
-        <v>4.416</v>
+        <v>4416</v>
       </c>
       <c r="M13" t="n">
-        <v>4.143</v>
+        <v>4143</v>
       </c>
       <c r="N13" t="n">
-        <v>49.77</v>
+        <v>49770</v>
       </c>
     </row>
     <row r="14">
@@ -1064,43 +1064,43 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2.722</v>
+        <v>2722</v>
       </c>
       <c r="C14" t="n">
-        <v>2.648</v>
+        <v>2648</v>
       </c>
       <c r="D14" t="n">
-        <v>2.792</v>
+        <v>2792</v>
       </c>
       <c r="E14" t="n">
-        <v>2.886</v>
+        <v>2886</v>
       </c>
       <c r="F14" t="n">
-        <v>2.973</v>
+        <v>2973</v>
       </c>
       <c r="G14" t="n">
-        <v>2.758</v>
+        <v>2758</v>
       </c>
       <c r="H14" t="n">
-        <v>2.861</v>
+        <v>2861</v>
       </c>
       <c r="I14" t="n">
-        <v>2.861</v>
+        <v>2861</v>
       </c>
       <c r="J14" t="n">
-        <v>2.751</v>
+        <v>2751</v>
       </c>
       <c r="K14" t="n">
-        <v>2.907</v>
+        <v>2907</v>
       </c>
       <c r="L14" t="n">
-        <v>2.71</v>
+        <v>2710</v>
       </c>
       <c r="M14" t="n">
-        <v>2.649</v>
+        <v>2649</v>
       </c>
       <c r="N14" t="n">
-        <v>33.518</v>
+        <v>33518</v>
       </c>
     </row>
     <row r="15">
@@ -1110,7 +1110,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1.232</v>
+        <v>1232</v>
       </c>
       <c r="C15" t="n">
         <v>982</v>
@@ -1119,34 +1119,34 @@
         <v>978</v>
       </c>
       <c r="E15" t="n">
-        <v>1.022</v>
+        <v>1022</v>
       </c>
       <c r="F15" t="n">
-        <v>1.081</v>
+        <v>1081</v>
       </c>
       <c r="G15" t="n">
         <v>865</v>
       </c>
       <c r="H15" t="n">
-        <v>1.056</v>
+        <v>1056</v>
       </c>
       <c r="I15" t="n">
-        <v>1.06</v>
+        <v>1060</v>
       </c>
       <c r="J15" t="n">
-        <v>1.022</v>
+        <v>1022</v>
       </c>
       <c r="K15" t="n">
-        <v>1.083</v>
+        <v>1083</v>
       </c>
       <c r="L15" t="n">
-        <v>1.161</v>
+        <v>1161</v>
       </c>
       <c r="M15" t="n">
-        <v>1.442</v>
+        <v>1442</v>
       </c>
       <c r="N15" t="n">
-        <v>2835.159</v>
+        <v>12984</v>
       </c>
     </row>
     <row r="16">
@@ -1162,37 +1162,37 @@
         <v>581</v>
       </c>
       <c r="D16" t="n">
-        <v>1.093</v>
+        <v>1093</v>
       </c>
       <c r="E16" t="n">
-        <v>1.218</v>
+        <v>1218</v>
       </c>
       <c r="F16" t="n">
         <v>947</v>
       </c>
       <c r="G16" t="n">
-        <v>1.181</v>
+        <v>1181</v>
       </c>
       <c r="H16" t="n">
-        <v>2.514</v>
+        <v>2514</v>
       </c>
       <c r="I16" t="n">
-        <v>2.906</v>
+        <v>2906</v>
       </c>
       <c r="J16" t="n">
-        <v>1.982</v>
+        <v>1982</v>
       </c>
       <c r="K16" t="n">
-        <v>1.695</v>
+        <v>1695</v>
       </c>
       <c r="L16" t="n">
-        <v>1.432</v>
+        <v>1432</v>
       </c>
       <c r="M16" t="n">
-        <v>1.263</v>
+        <v>1263</v>
       </c>
       <c r="N16" t="n">
-        <v>2538.284</v>
+        <v>17807</v>
       </c>
     </row>
     <row r="17">
@@ -1453,22 +1453,22 @@
         <v>52</v>
       </c>
       <c r="I22" t="n">
-        <v>2.85</v>
+        <v>2850</v>
       </c>
       <c r="J22" t="n">
-        <v>2.007</v>
+        <v>2007</v>
       </c>
       <c r="K22" t="n">
-        <v>2.352</v>
+        <v>2352</v>
       </c>
       <c r="L22" t="n">
-        <v>2.287</v>
+        <v>2287</v>
       </c>
       <c r="M22" t="n">
-        <v>2.544</v>
+        <v>2544</v>
       </c>
       <c r="N22" t="n">
-        <v>64.03999999999999</v>
+        <v>12092</v>
       </c>
     </row>
     <row r="23">

</xml_diff>